<commit_message>
Abrir imagem da galeria - Porem nao salva
</commit_message>
<xml_diff>
--- a/CoresApp.xlsx
+++ b/CoresApp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reserva\Documents\GitHub\praticarAndroidStudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47CA8F6-9626-4327-AF6E-E33E5F7421BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608372E2-C0B5-487F-AB34-5A1888EA6BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2100" windowWidth="20730" windowHeight="11160" xr2:uid="{775FA168-B112-46CB-8FA5-CE68E526E267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{775FA168-B112-46CB-8FA5-CE68E526E267}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Darkmode</t>
   </si>
@@ -64,13 +64,19 @@
   </si>
   <si>
     <t>#F29BAB</t>
+  </si>
+  <si>
+    <t>#010238</t>
+  </si>
+  <si>
+    <t>corDark03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +98,14 @@
       <color rgb="FF486830"/>
       <name val="JetBrains Mono"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +133,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF732735"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF010238"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -149,6 +167,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,6 +176,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF010238"/>
       <color rgb="FFF29BAB"/>
       <color rgb="FF96D2D9"/>
       <color rgb="FF732735"/>
@@ -471,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921ADB2A-322D-47A7-B3DE-5E00C7E8D576}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,11 +549,22 @@
       </c>
       <c r="F3" s="3"/>
     </row>
+    <row r="4" spans="1:6" ht="15.75">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>